<commit_message>
Windows Compatible version in arddata change to the port connected to arduino
</commit_message>
<xml_diff>
--- a/IOT_SEC_A.xlsx
+++ b/IOT_SEC_A.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17480" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,17 +412,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="1" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -439,7 +436,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>43 TR IO TD</t>
+          <t>43 TR IO TW</t>
         </is>
       </c>
     </row>
@@ -456,7 +453,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>43 TR IO TD</t>
+          <t>43 TR IO TW</t>
         </is>
       </c>
     </row>
@@ -473,7 +470,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>43 TR IO TD</t>
+          <t>43 TR IO TW</t>
         </is>
       </c>
     </row>
@@ -490,7 +487,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>43 TR IO TD</t>
+          <t>43 TR IO TW</t>
         </is>
       </c>
     </row>
@@ -525,6 +522,108 @@
       <c r="C6" t="inlineStr">
         <is>
           <t>43 TR IO TD</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LOVE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>219311046</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>43 TR IO TD</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LOVE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>219311046</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>43 TR IO TD</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>LOVE</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>219311046</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>43 TR IO TD</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LOVE</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>219311046</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>43 TR IO TD</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Love Lakhwani</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>219311046</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1D 72 B0 04</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Utkarsh Triphati</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>211015048</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>AD B2 D3 04</t>
         </is>
       </c>
     </row>

</xml_diff>